<commit_message>
update tag recapture data
</commit_message>
<xml_diff>
--- a/data/taggingData/tagRecaptures.xlsx
+++ b/data/taggingData/tagRecaptures.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>fish</t>
   </si>
@@ -92,9 +92,6 @@
     <t>794 South A Street, Washougle WA, 98671</t>
   </si>
   <si>
-    <t>Hood Canal area</t>
-  </si>
-  <si>
     <t>CK118</t>
   </si>
   <si>
@@ -129,6 +126,24 @@
   </si>
   <si>
     <t>sport</t>
+  </si>
+  <si>
+    <t>no tag number; acoustic tag missing</t>
+  </si>
+  <si>
+    <t>Lower Harrison Reiver</t>
+  </si>
+  <si>
+    <t>Sts'ailes</t>
+  </si>
+  <si>
+    <t>Kim Charlie</t>
+  </si>
+  <si>
+    <t>4690 Salish Way, Agassiz BC, V0M1A1</t>
+  </si>
+  <si>
+    <t>Hood Canal</t>
   </si>
 </sst>
 </file>
@@ -458,7 +473,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
@@ -489,13 +504,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>32</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
@@ -513,7 +528,7 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -523,20 +538,20 @@
       <c r="B2">
         <v>7730</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
+      <c r="C2" s="2">
+        <v>43705</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
+        <v>39</v>
+      </c>
+      <c r="E2">
+        <v>47.407499000000001</v>
+      </c>
+      <c r="F2">
+        <v>-123.136264</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
@@ -574,7 +589,7 @@
         <v>-123.11790000000001</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
         <v>7</v>
@@ -612,7 +627,7 @@
         <v>-122.33669999999999</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
         <v>19</v>
@@ -632,7 +647,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>7738</v>
@@ -641,7 +656,7 @@
         <v>43708</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5">
         <v>47.179876999999998</v>
@@ -650,13 +665,13 @@
         <v>-122.922578</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
         <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>26</v>
       </c>
       <c r="J5">
         <v>13604630765</v>
@@ -665,10 +680,51 @@
         <v>6</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M5" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43707</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6">
+        <v>49.251817000000003</v>
+      </c>
+      <c r="F6">
+        <v>-121.93721499999999</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6">
+        <v>16047962116</v>
+      </c>
+      <c r="K6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with returned tag
</commit_message>
<xml_diff>
--- a/data/taggingData/tagRecaptures.xlsx
+++ b/data/taggingData/tagRecaptures.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>fish</t>
   </si>
@@ -536,7 +536,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -841,6 +841,9 @@
       <c r="B8">
         <v>7715</v>
       </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
       <c r="D8" s="2">
         <v>43697</v>
       </c>

</xml_diff>